<commit_message>
Nurse Registratsiya bo'limi 100% foiz tayor test qilindi
</commit_message>
<xml_diff>
--- a/Bemorlar ro`yxati.xlsx
+++ b/Bemorlar ro`yxati.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t xml:space="preserve">ID raqami </t>
   </si>
@@ -51,6 +51,24 @@
   </si>
   <si>
     <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Asal</t>
+  </si>
+  <si>
+    <t>+998909999999</t>
+  </si>
+  <si>
+    <t>1qavat</t>
+  </si>
+  <si>
+    <t>21xona</t>
+  </si>
+  <si>
+    <t>2022-12-07</t>
   </si>
 </sst>
 </file>
@@ -95,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -147,6 +165,29 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>